<commit_message>
Add README for model fine-tuning and update evaluation results
Introduced a detailed README outlining setup, requirements, and usage of the fine-tuning script for QWEN2.5-7B. Additionally, updated evaluation results stored in the referenced Excel file for better analysis.
</commit_message>
<xml_diff>
--- a/Eval/Results_Checkpoint_Model_Short.xlsx
+++ b/Eval/Results_Checkpoint_Model_Short.xlsx
@@ -20909,7 +20909,221 @@
           <t>Physics</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr"/>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>&lt;|im_start|&gt;think
+Let $R$ be the radius of the detector, $r_0$ be the initial position of the particle inside the detector, $\gamma$ be the Lorentz factor, and $c$ be the speed of light.
+The velocity of the particles is $v = c/\gamma$.
+The particles travel uninterrupted at ultra-relativistic velocities, so we can assume $v \approx c$.
+The particles decay while traveling.
+The mean distance traveled by a particle before decaying is given by $\frac{1}{\Gamma(1)} = \frac{1}{\lambda}$, where $\lambda$ is the decay constant.
+The probability that a particle survives and travels a distance $d$ is $e^{-d/\lambda}$.
+Here, the distance $d$ is the radius of the detector $R$.
+The probability that a particle reaches the detector inner walls is $e^{-R/\lambda}$.
+We are given that on average, one third of these fast-decaying particles reaches the detector inner walls.
+So, $e^{-R/\lambda} = 1/3$.
+We need to find the Lorentz factor $\gamma$ such that about two thirds of these particles reach the detector inner walls.
+The probability that a particle reaches the detector inner walls is $e^{-R/\lambda'}$, where $\lambda'$ is the effective decay constant in the lab frame.
+Due to time dilation, the decay constant in the lab frame is related to the decay constant in the particle's rest frame by $\lambda' = \gamma \lambda$.
+The probability that a particle reaches the detector inner walls in the lab frame is $e^{-R/\lambda'} = e^{-R/( \gamma \lambda )}$.
+We want this probability to be $2/3$.
+So, $e^{-R/( \gamma \lambda )} = 2/3$.
+We have $e^{-R/\lambda} = 1/3$. Let $k = R/\lambda$. Then $e^{-k} = 1/3$.
+We want $e^{-k'/\gamma} = 2/3$, where $k' = R/\lambda'$. Since $\lambda' = \lambda$, $k' = k$.
+This seems wrong. Let's rethink the problem.
+The mean distance traveled by a particle before decaying is $\frac{1}{\lambda}$. This is in the rest frame of the particle.
+In the lab frame, due to time dilation, the decay process happens slower. The effective decay constant is $\lambda' = \gamma \lambda$.
+The mean distance traveled by a particle before decaying in the lab frame is $\frac{1}{\lambda'} = \frac{1}{\gamma \lambda}$.
+The probability that a particle travels a distance $R$ before decaying in the lab frame is $e^{-R / (\gamma \lambda)}$.
+We are given that in the rest frame of the particles (where they are produced), one third reach the walls. This means the mean distance they can travel before decaying is at least the radius of the detector.
+So, $\frac{1}{\lambda} \ge R$.
+Now, consider the lab frame. We want two thirds of the particles to reach the inner walls.
+The probability of a single particle reaching the walls is $e^{-R / (\gamma \lambda)}$.
+If the particles were independent and the decay was instantaneous, the number of particles reaching the walls would follow a binomial distribution. However, the decay is continuous.
+Let the number of particles produced be $N$. The number of particles reaching the walls follows a Poisson distribution with mean $\lambda_{eff} N$, where $\lambda_{eff}$ is the effective decay constant in the lab frame.
+The probability that a particle reaches the walls is $1 - e^{-R / (\gamma \lambda)}$.
+Let $P_{reach} = 2/3$.
+$1 - e^{-R / (\gamma \lambda)} = 2/3$
+$e^{-R / (\gamma \lambda)} = 1/3$
+$-R / (\gamma \lambda) = \ln(1/3) = -\ln(3)$
+$R / (\gamma \lambda) = \ln(3)$
+We are given $R = 30$ meters.
+We need to find $\gamma$.
+From the first part, we know that in the rest frame, one third reach the walls, so $e^{-30/\lambda} = 1/3$.
+$30/\lambda = \ln(3)$.
+So, $\lambda = 30 / \ln(3)$.
+Substitute this into the equation for the lab frame:
+$30 / (\gamma \times (30 / \ln(3))) = \ln(3)$
+$30 \ln(3) / (30 \gamma) = \ln(3)$
+$\ln(3) / \gamma = \ln(3)$
+$\gamma = 1$.
+Let's re-examine the meaning of "one third of these fast-decaying particles reaches the detector inner walls". This means the survival probability is $1/3$.
+The probability that a particle survives until it reaches a distance $R$ is $e^{-R/\lambda_{rest}} = 1/3$.
+So, $\lambda_{rest} = R / \ln(3)$.
+Now consider the lab frame. The decay constant is $\lambda_{lab} = \gamma \lambda_{rest}$.
+The probability that a particle is found within the detector radius $R$ is $e^{-R/\lambda_{lab}}$.
+We want this probability to be $2/3$.
+$e^{-R/( \gamma \lambda_{rest} )} = 2/3$
+$e^{-R/( \gamma (R/\ln(3)) )} = 2/3$
+$e^{-\ln(3)/\gamma} = 2/3$
+$-\ln(3)/\gamma = \ln(2/3) = \ln(2) - \ln(3)$
+$\ln(3)/\gamma = \ln(3) - \ln(2)$
+$\gamma = \frac{\ln(3)}{\ln(3) - \ln(2)} = \frac{\ln(3)}{\ln(3/2)}$
+$\gamma = \frac{\ln(3)}{\ln(3) - \ln(2)} = \frac{1.0986}{1.0986 - 0.6931} = \frac{1.0986}{0.4055} \approx 2.711$.
+Let's check the conditions.
+In the rest frame, $\lambda = R / \ln(3)$. The mean distance traveled is $\frac{1}{\lambda} = \ln(3)/R$. If this is greater than or equal to $R$, it means almost no particles reach the wall. Something is wrong.
+The interpretation of "one third of these fast-decaying particles reaches the detector inner walls" is the probability of a particle reaching the walls is $1/3$.
+So, $e^{-R/\lambda_{rest}} = 1/3$.
+The Lorentz factor affects the decay rate. The mean lifetime in the lab frame is $\tau' = \gamma \tau$, where $\tau$ is the proper lifetime (in the rest frame).
+The mean distance traveled in the rest frame before decaying is $v \tau = c \tau / \gamma$.
+The mean distance is also $1/\lambda_{rest}$.
+So, $c \tau_{rest} / \gamma = 1/\lambda_{rest}$.
+$\tau_{rest} = \gamma \lambda_{rest}$.
+The probability that a particle reaches the wall in the rest frame is the probability that its lifetime is greater than the distance to the wall divided by its speed. This is $e^{-R v/\lambda_{rest}} = e^{-R c/\gamma \lambda_{rest}}$.
+We are given that this probability is $1/3$.
+$e^{-R c/( \gamma \lambda_{rest} )} = 1/3$
+$-R c / ( \gamma \lambda_{rest} ) = \ln(1/3) = -\ln(3)$
+$R c / ( \gamma \lambda_{rest} ) = \ln(3)$
+$R / \gamma \lambda_{rest} = \ln(3) / c$
+Since we are considering the conditions in the rest frame where the particles are produced, the decay constant is $\lambda_{rest}$.
+Now consider the lab frame. We want the probability of a particle reaching the walls to be $2/3$.
+The mean distance traveled by a particle before decaying in the lab frame is $1/\lambda_{lab} = \gamma \lambda_{rest}$.
+The probability that a particle travels a distance $R$ before decaying is $e^{-R/\lambda_{lab}}$.
+We want $e^{-R/\lambda_{lab}} = 2/3$.
+$e^{-R/( \gamma \lambda_{rest} )} = 2/3$
+$-R / ( \gamma \lambda_{rest} ) = \ln(2/3) = \ln(2) - \ln(3)$
+$R / ( \gamma \lambda_{rest} ) = \ln(3) - \ln(2)$
+We know $R = 30$ meters.
+$\gamma \lambda_{rest} = \frac{R}{\ln(3) - \ln(2)} = \frac{30}{\ln(3) - \ln(2)} = \frac{30}{\ln(3/2)}$.
+We need to find $\gamma$.
+From the rest frame condition, $e^{-30/\lambda_{rest}} = 1/3$, so $\lambda_{rest} = 30 / \ln(3)$.
+Substitute this into the lab frame equation:
+$\gamma \times \frac{30}{\ln(3)} = \frac{30}{\ln(3/2)}$
+$\gamma = \frac{\ln(3/2)}{\ln(3)} = \frac{\ln(3) - \ln(2)}{\ln(3)} = 1 - \frac{\ln(2)}{\ln(3)} = 1 - \log_3(2)$.
+$\log_3(2) = \frac{\ln(2)}{\ln(3)} \approx \frac{0.6931}{1.0986} \approx 0.63$.
+$\gamma = 1 - 0.63 = 0.37$.
+Let's think about the physics. The decay rate is observed to be slower due to time dilation.
+The mean lifetime in the lab frame is $\tau' = \gamma \tau$.
+The mean distance traveled before decaying in the lab frame is $v \tau' = c \tau / \gamma$.
+The probability that a particle reaches the walls is $e^{-R v/\lambda_{eff}}$, where $\lambda_{eff}$ is the effective decay constant in the lab frame.
+The number of particles produced per unit time is $N_0$. The number reaching the walls follows a Poisson distribution with mean rate $\lambda_{eff} N_0$.
+The probability that a single particle reaches the walls is $1 - e^{-R/\lambda_{eff}}$.
+We want this probability to be $2/3$.
+$1 - e^{-R/\lambda_{eff}} = 2/3$
+$e^{-R/\lambda_{eff}} = 1/3$
+$-R/\lambda_{eff} = \ln(1/3) = -\ln(3)$
+$\lambda_{eff} = R/\ln(3)$.
+The effective decay constant in the lab frame is $\lambda' = \gamma \lambda_{rest}$.
+So, $R/\ln(3) = \gamma \lambda_{rest}$.
+We are given that in the rest frame, one third reach the walls, so $e^{-R/\lambda_{rest}} = 1/3$, which means $\lambda_{rest} = R/\ln(3)$.
+Substituting this back into the equation for $\lambda_{eff}$:
+$R/\ln(3) = \gamma (R/\ln(3))$
+$\gamma = 1$.
+This contradicts the previous result.
+Let's consider the flux of particles reaching the walls.
+The rate of particles produced is $R_0$. The rate of particles reaching the walls is $R_0 \times (probability)$.
+In the rest frame, the probability is $1/3$.
+In the lab frame, the probability is $2/3$.
+The number of particles produced per unit time is the same.
+Let the number of particles produced be $N$.
+The number reaching the walls in the rest frame is $N/3$.
+The number reaching the walls in the lab frame is $(2/3) N$.
+The mean distance traveled before decaying is related to the decay constant.
+Consider a single particle. The probability it reaches the walls is $e^{-R/\lambda_{rest}} = 1/3$.
+In the lab frame, the effective decay constant is $\lambda' = \gamma \lambda_{rest}$.
+The probability a particle reaches the walls is $e^{-R/\lambda'} = e^{-R/( \gamma \lambda_{rest} )}$.
+We want this to be $2/3$.
+$e^{-R/( \gamma \lambda_{rest} )} = 2/3$
+$-R / ( \gamma \lambda_{rest} ) = \ln(2/3)$
+$R / ( \gamma \lambda_{rest} ) = \ln(3/2)$
+$30 / ( \gamma \times 30 / \ln(3) ) = \ln(3/2)$
+$\ln(3) / \gamma = \ln(3/2)$
+$\gamma = \ln(3) / \ln(3/2) = \ln(3) / (\ln(3) - \ln(2)) \approx 1.0986 / 0.4055 \approx 2.71$.
+Let's trust the calculation with the probability approach.
+The probability that a particle survives until it is within a distance $R$ is $e^{-R/\lambda_{rest}}$.
+The probability that a particle reaches the walls is the probability that its lifetime is greater than the time to travel $R$ at speed $c/\gamma$.
+$e^{-R v/\lambda_{rest}} = e^{-R c/( \gamma \lambda_{rest} )} = 1/3$.
+Now, in the lab frame, the effective decay constant is $\lambda' = \gamma \lambda_{rest}$.
+The probability that a particle is found within the detector radius $R$ is $e^{-R/\lambda'} = e^{-R/( \gamma \lambda_{rest} )}$.
+We want this probability to be $2/3$.
+$e^{-R/( \gamma \lambda_{rest} )} = 2/3$.
+We found $\lambda_{rest}$ from the first condition.
+The question implies that the Lorentz factor needs to be changed to affect the number of particles reaching the walls. This suggests the decay rate is observed differently in the lab frame due to the motion of the particles.
+The proper decay constant is $\lambda_{rest}$. The lab frame observes a dilated decay constant $\lambda' = \gamma \lambda_{rest}$.
+The probability of surviving until time $t$ in the rest frame is $e^{-t/\lambda_{rest}}$.
+The probability of surviving until time $\gamma T$ (the lifetime in the lab frame) is $e^{-\gamma T / \lambda_{rest}}$.
+If the particles are produced at time $t=0$, the probability that a particle is detected within the detector's lifetime is related to the decay process.
+The mean distance traveled before decaying in the rest frame is $\frac{c}{\gamma} \tau_{rest} = \frac{1}{\lambda_{rest}}$.
+The probability that a particle reaches the walls is $e^{-R/\lambda_{rest}} = 1/3$.
+In the lab frame, the effective decay constant is $\lambda' = \gamma \lambda_{rest}$.
+The probability that a particle is found within the radius $R$ is $e^{-R/\lambda'} = e^{-R/( \gamma \lambda_{rest} )}$.
+We want this probability to be $2/3$.
+$e^{-30/( \gamma \times 30 / \ln(3) )} = 2/3$
+$e^{-\ln(3)/\gamma} = 2/3$
+$-\ln(3)/\gamma = \ln(2/3)$
+$\gamma = -\frac{\ln(3)}{\ln(2/3)} = \frac{\ln(3)}{1 - \ln(3)} = \frac{1.0986}{1 - 1.0986} = \frac{1.0986}{-0.0986} \approx -11.1$.
+This negative value indicates an error in interpretation.
+The probability that a particle reaches the walls is the probability that its lifetime is longer than the time it takes to travel $R$.
+In the rest frame, this probability is $1/3$.
+In the lab frame, due to time dilation, the decay process appears slower, increasing the probability of reaching the walls.
+The effective decay constant in the lab frame is $\lambda' = \gamma \lambda_{rest}$.
+The probability that a particle reaches the walls is $1 - e^{-R/\lambda'} = 2/3$.
+$e^{-R/\lambda'} = 1/3$.
+$-R/\lambda' = \ln(1/3) = -\ln(3)$.
+$\lambda' = R/\ln(3)$.
+$\gamma \lambda_{rest} = R/\ln(3)$.
+From the rest frame condition, $e^{-R/\lambda_{rest}} = 1/3$, so $\lambda_{rest} = R/\ln(3)$.
+Substituting, $\gamma \times R/\ln(3) = R/\ln(3)$, so $\gamma = 1$.
+This still gives $\gamma=1$. Let's reconsider the wording.
+"What Lorentz factor is needed in order to have about two thirds of these fast-decaying particles reaching the detector inner walls?"
+The Lorentz factor affects the decay rate as observed in the lab frame.
+The proper decay constant is $\lambda_{rest}$. The lab frame observes $\lambda' = \gamma \lambda_{rest}$.
+The probability of a particle reaching the walls in the lab frame is related to the effective decay constant.
+If the Lorentz factor is $\gamma$, the observed decay constant is larger, leading to a higher probability of the particles decaying after traveling a certain distance.
+The probability that a particle reaches the walls in the rest frame is $P_{rest} = 1/3$.
+The probability that a particle reaches the walls in the lab frame is $P_{lab} = 2/3$.
+The relationship between the probabilities needs to be consistent with the time dilation.
+The time for a particle to decay is $\tau' = \gamma \tau$.
+The distance traveled is $v \tau' = c \tau / \gamma$.
+The probability that a particle reaches the walls is $e^{-R v/\lambda_{eff}}$.
+In the rest frame, $\lambda_{eff} = \lambda_{rest}$. $e^{-R/c \lambda_{rest}} = 1/3$.
+In the lab frame, $\lambda' = \gamma \lambda_{rest}$. $e^{-R/c \lambda'} = e^{-R/( \gamma \lambda_{rest} )} = 2/3$.
+From the first equation, $R / (c \lambda_{rest}) = \ln(3)$.
+Substitute into the second: $e^{-\ln(3) \gamma} = 2/3$.
+$-\ln(3) \gamma = \ln(2/3)$.
+$\gamma = -\frac{\ln(2/3)}{\ln(3)} = \frac{\ln(3) - \ln(2)}{\ln(3)} = 1 - \frac{\ln(2)}{\ln(3)} = 1 - \log_3(2) \approx 1 - 0.63 = 0.37$.
+The Lorentz factor needs to be smaller than 1 for the probability to increase. This implies a slower moving particle, which contradicts the ultra-relativistic velocity assumption.
+The phrase "Lorentz factor of ~20" refers to the particles themselves, not the detection probability. The decay rate of the particles is observed to be faster in the rest frame.
+The probability calculation seems correct. The Lorentz factor acts to effective slow down the decay process in the lab frame, increasing the probability of reaching the walls.
+Final check:
+Rest frame: $e^{-R/\lambda} = 1/3 \implies \lambda = R \ln(3)$.
+Lab frame: $e^{-R/\lambda'} = 2/3$, where $\lambda' = \gamma \lambda = \gamma R \ln(3)$.
+$e^{-R/( \gamma R \ln(3) )} = 2/3$.
+$e^{-1/( \gamma \ln(3) )} = 2/3$.
+$-\frac{1}{\gamma \ln(3)} = \ln(2/3)$.
+$\gamma = -\frac{1}{\ln(3) \ln(2/3)} = \frac{1}{\ln(3) (\ln(3) - \ln(2))} = \frac{1}{\ln(3) / \ln(3/2)} = \ln(3/2) / \ln(3) = 1 - \ln(2)/\ln(3)$.
+&lt;|im_start|&gt;answer
+Solution:
+Let $R$ be the radius of the detector, $v$ be the velocity of the particles, and $\gamma$ be the Lorentz factor. The velocity of the particles is $v = c/\gamma$, where $c$ is the speed of light. The mean distance traveled by a particle before decaying is $1/\lambda_{rest}$ in the rest frame of the particles.
+We are given that in the rest frame of the particles, one third reach the detector inner walls. This means the probability that a particle travels a distance $R$ before decaying is $1/3$.
+$e^{-R/\lambda_{rest}} = 1/3$
+$R/\lambda_{rest} = \ln(3)$
+$\lambda_{rest} = R/\ln(3)$
+In the lab frame, due to time dilation, the decay constant is $\lambda' = \gamma \lambda_{rest}$.
+The probability that a particle reaches the detector inner walls in the lab frame is about two thirds. This means the probability that a particle travels a distance $R$ before decaying in the lab frame is $2/3$.
+$e^{-R/\lambda'} = 2/3$
+$e^{-R/( \gamma \lambda_{rest} )} = 2/3$
+$e^{-R/( \gamma (R/\ln(3)) )} = 2/3$
+$e^{-\ln(3)/\gamma} = 2/3$
+$-\ln(3)/\gamma = \ln(2/3)$
+$\gamma = -\frac{\ln(3)}{\ln(2/3)} = \frac{\ln(3) - \ln(2)}{\ln(3)} = 1 - \frac{\ln(2)}{\ln(3)}$
+Calculating the numerical value:
+$\ln(2) \approx 0.6931$
+$\ln(3) \approx 1.0986$
+$\gamma = 1 - \frac{0.6931}{1.0986} \approx 1 - 0.6300 \approx 0.3700$
+Final Answer: The final answer is $\boxed{0.37}$</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -20930,7 +21144,69 @@
           <t>Physics</t>
         </is>
       </c>
-      <c r="E126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>&lt;|im_start|&gt;think
+The problem asks for the energy of the third excited state and the number of linearly independent eigenfunctions for that energy in a quantum harmonic oscillator in three dimensions.
+The potential is given by $V(r) = \frac{1}{2} m \omega^2 r^2$. This is the potential for a 3D harmonic oscillator.
+The energy levels of a 3D harmonic oscillator are given by $E_{n_1 n_2 n_3} = \hbar \omega (n_1 + n_2 + n_3 + \frac{3}{2})$, where $n_1, n_2, n_3$ are non-negative integers ($0, 1, 2, \dots$).
+The energy eigenvalues can be written in terms of the total quantum number $N = n_1 + n_2 + n_3$. The possible values of $N$ are $0, 1, 2, \dots$.
+For a given $N$, the number of possible sets of $(n_1, n_2, n_3)$ such that $n_1 + n_2 + n_3 = N$ is the number of ways to distribute $N$ identical items into 3 distinct bins, which is $\binom{N+3-1}{3-1} = \binom{N+2}{2}$.
+The energy levels are $E_N = \hbar \omega (N + \frac{3}{2})$.
+The energy of the $k$-th excited state corresponds to $N = k$.
+The third excited state corresponds to $N = 3$.
+The energy of the third excited state is $E_3 = \hbar \omega (3 + \frac{3}{2}) = \hbar \omega (\frac{6}{2} + \frac{3}{2}) = \hbar \omega \frac{9}{2}$.
+Now, we need to find the number of linearly independent eigenfunctions for the energy eigenvalue $E_3$.
+For $E_3$, we have $N=3$. The possible sets of $(n_1, n_2, n_3)$ such that $n_1 + n_2 + n_3 = 3$ are:
+(n_1, n_2, n_3) = (3, 0, 0), (0, 3, 0), (0, 0, 3)
+(n_1, n_2, n_3) = (2, 1, 0), (2, 0, 1), (1, 2, 0), (1, 0, 2), (0, 2, 1), (0, 1, 2)
+(n_1, n_2, n_3) = (1, 1, 1)
+The number of linearly independent eigenfunctions for a given energy eigenvalue $E_N$ is the number of non-negative integer solutions to the equation $n_1 + n_2 + n_3 = N$. This is $\binom{N+2}{2}$.
+For $N=3$, the number of linearly independent eigenfunctions is $\binom{3+2}{2} = \binom{5}{2} = \frac{5 \times 4}{2 \times 1} = 10$.
+Alternatively, we can list them explicitly. The eigenfunctions are proportional to $e^{-\alpha r^2/2} L_n^{(\alpha-1)}(r^2) P_{n_1}(\cos \theta) e^{i m \phi}$, where $\alpha = m \omega / \hbar$. For a spherical potential, the angular part of the wavefunction is independent of $\phi$, so $m=0$. The radial part is proportional to $R_{n_1 n_2 n_3}(r)$.
+The number of linearly independent eigenfunctions for a given energy is the number of ways to form a set of non-negative integers $(n_1, n_2, n_3)$ that sum to $N$. This is the partitions of $N$ into at most 3 parts.
+Partitions of 3 into at most 3 parts:
+3
+2, 1
+1, 1, 1
+The number of parts is related to the number of terms in the sum. Here, we have three terms $n_1, n_2, n_3$.
+Let's consider the number of solutions to $x_1 + x_2 + \dots + x_k = N$, where $x_i \ge 0$. This is $\binom{N+k-1}{k-1}$.
+For our case, $k=3$. The number of solutions to $n_1 + n_2 + n_3 = 3$ is $\binom{3+3-1}{3-1} = \binom{5}{2} = 10$.
+The energy of the third excited state is $E_3 = \frac{9}{2} \hbar \omega$.
+The number of linearly independent eigenfunctions for this energy is 10.
+Let's double-check the concept of excited states. The ground state has $N=0$, so $E_0 = \frac{3}{2} \hbar \omega$. The first excited state has $N=1$, so $E_1 = \frac{5}{2} \hbar \omega$. The second excited state has $N=2$, so $E_2 = \frac{7}{2} \hbar \omega$. The third excited state has $N=3$, so $E_3 = \frac{9}{2} \hbar \omega$.
+For $N=3$, the possible sets of $(n_1, n_2, n_3)$ are:
+(3, 0, 0) -&gt; $e^{-\alpha r^2/2} L_3^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(0, 3, 0) -&gt; $e^{-\alpha r^2/2} L_3^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(0, 0, 3) -&gt; $e^{-\alpha r^2/2} L_3^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(2, 1, 0) -&gt; $e^{-\alpha r^2/2} L_2^{(\alpha-1)}(r^2) L_1^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(2, 0, 1) -&gt; $e^{-\alpha r^2/2} L_2^{(\alpha-1)}(r^2) L_1^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(1, 2, 0) -&gt; $e^{-\alpha r^2/2} L_1^{(\alpha-1)}(r^2) L_2^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(1, 0, 2) -&gt; $e^{-\alpha r^2/2} L_1^{(\alpha-1)}(r^2) L_2^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(0, 2, 1) -&gt; $e^{-\alpha r^2/2} L_3^{(\alpha-1)}(r^2) L_1^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(0, 1, 2) -&gt; $e^{-\alpha r^2/2} L_3^{(\alpha-1)}(r^2) L_1^{(\alpha-1)}(r^2) Y_0^0(\theta, \phi)$
+(1, 1, 1) -&gt; $e^{-\alpha r^2/2} L_1^{(\alpha-1)}(r^2)^3 Y_0^0(\theta, \phi)$
+The number of these combinations is 10. Each combination corresponds to a set of quantum numbers $(n_1, n_2, n_3)$ that gives the same energy $E_3$.
+The eigenfunctions for a given energy eigenvalue are the orthogonalized versions of these solutions.
+Final check of the question: "What is the value of energy of the third excited state?" and "how many linearly independent eigenfunctions are possible for the same energy eigenvalue?"
+Energy of the third excited state: $E_3 = \frac{9}{2} \hbar \omega$.
+Number of linearly independent eigenfunctions for $E_3$: 10.
+The question implies that all these 10 eigenfunctions are linearly independent of each other for the same energy eigenvalue $E_3$.
+&lt;|im_start|&gt;answer
+The energy levels of a particle in a three-dimensional isotropic harmonic potential $V(r) = \frac{1}{2} m \omega^2 r^2$ are given by $E_{n_1 n_2 n_3} = \hbar \omega (n_1 + n_2 + n_3 + \frac{3}{2})$, where $n_1, n_2, n_3$ are non-negative integers ($0, 1, 2, \dots$).
+The energy of the $k$-th excited state corresponds to $N = k$, where $N = n_1 + n_2 + n_3$. The energy of the third excited state corresponds to $N = 3$.
+The energy of the third excited state is $E_3 = \hbar \omega (3 + \frac{3}{2}) = \hbar \omega \frac{9}{2}$.
+The number of linearly independent eigenfunctions for a given energy eigenvalue $E_N$ is the number of sets of non-negative integers $(n_1, n_2, n_3)$ such that $n_1 + n_2 + n_3 = N$. This is equivalent to the number of ways to distribute $N$ identical items into 3 distinct bins, which is given by the binomial coefficient $\binom{N+3-1}{3-1} = \binom{N+2}{2}$.
+For $N=3$, the number of linearly independent eigenfunctions is $\binom{3+2}{2} = \binom{5}{2} = \frac{5 \times 4}{2 \times 1} = 10$.
+Alternatively, we can list the possible sets of $(n_1, n_2, n_3)$ such that $n_1 + n_2 + n_3 = 3$:
+(3, 0, 0), (0, 3, 0), (0, 0, 3)
+(2, 1, 0), (2, 0, 1), (1, 2, 0), (1, 0, 2), (0, 2, 1), (0, 1, 2)
+(1, 1, 1)
+There are 10 such sets, corresponding to 10 linearly independent eigenfunctions.
+The eigenfunctions for a given energy eigenvalue are orthogonal to each other. Therefore, the number of linearly independent eigenfunctions for the same energy eigenvalue is equal to the number of different sets of quantum numbers $(n_1, n_2, n_3)$ that give that energy.
+Final Answer: The final answer is $\boxed{E_{3} = \frac{9}{2} \hbar \omega, 10}$</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -20957,7 +21233,141 @@
           <t>Chemistry</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr"/>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>&lt;|im_start|&gt;think
+Let's break down each reaction and predict the products.
+**Reaction I: (S)-5-methoxyhexan-3-one with LAH and acidic workup**
+1. **LAH Treatment:**  LAH is a strong reducing agent. It reduces carbonyl groups (aldehydes and ketones) to alcohols. The (S)-5-methoxyhexan-3-one has a ketone at the C3 position. LAH will reduce this ketone to a primary alcohol.
+   The resulting alcohol will have the (S) configuration at the C3 position because the reduction step is stereospecific. The methoxy group (-OCH3) is a strong *ortho/para*-directing group, but since the reduction occurs at the C3 position, it won't significantly influence the stereochemistry at the reduction site. The resulting alcohol will retain the (S) configuration at C3.
+2. **Acidic Workup:**  The acidic workup will protonate the hydroxyl group to form a carbocation intermediate at the C3 position. This carbocation is allylic, as there is a conjugated double bond adjacent to the positive charge. Allylic carbocations are generally stable.
+   The key here is to consider the stereochemistry. The (S) alcohol will form a (S) carbocation upon protonation. The resulting carbocation will be planar due to the conjugated system.
+Let's consider the structure of the product from Reaction I:
+(S)-5-methoxy-3-hydroxyhexane, after reduction, becomes (S)-5-methoxy-3-hydroxycaproic acid upon acidic workup.
+**Reaction II: Pentane-2,4-dione with excess NaBH4 and acidic workup**
+1. **NaBH4 Treatment:** NaBH4 is a reducing agent that reduces carbonyl groups to alcohols. Pentane-2,4-dione has two carbonyl groups (a ketone at C2 and a ketone at C4). Both will be reduced to primary alcohols.
+   The reduction is stereospecific. The *endo* rule often applies in reductions like this, meaning that the hydrogen addition will occur on the same side as the larger substituent, if possible. However, in this case, the substituents are symmetrical. Let's consider the stereochemistry at each carbon:
+   - **C2:** The original group was -C(=O)-CH(CH3)2. After reduction, it becomes -CH(OH)-CH(CH3)2. The stereochemistry at C2 of the dione is *trans* to the methyl groups. After reduction, the hydroxyl group can rotate. For simplicity in predicting the *endo* product, we can assume the hydroxyl group adds *syn* to the larger group, which in this case is the methyl substituent. So, the *endo* product at C2 would have the hydroxyl group on the same face as one of the methyl groups. The *exo* product would have the hydroxyl group on the opposite face.
+   - **C4:** The original group was -CH(CH3)2-C(=O)-. After reduction, it becomes -CH(CH3)2-CH(OH)-. The stereochemistry at C4 of the dione is *trans* to the methyl groups. Similar to C2, the *endo* product at C4 will have the hydroxyl group on the same face as one of the methyl groups. The *exo* product would have the hydroxyl group on the opposite face.
+   Since the starting material is pentane-2,4-dione, the reduction will yield a mixture of *endo* and *exo* products at both the C2 and C4 positions.
+2. **Acidic Workup:**  The acidic workup will protonate the hydroxyl groups to form carbocation intermediates at the C2 and C4 positions. These carbocations are secondary carbocations.
+   Let's consider the possible products from Reaction II:
+   - **If both reductions are *endo*:**  The product would be (2S,4S)-1-hydroxy-2,4-dihydroxypentane. After acidic workup, this becomes (2S,4S)-1-hydroxy-2,4-dihydroxypentanoic acid.
+   - **If both reductions are *exo*:** The product would be (2R,4R)-1-hydroxy-2,4-dihydroxypentane. After acidic workup, this becomes (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid.
+   - **One *endo* and one *exo*:**  This would result in a meso compound if the configurations are opposite at the two centers. If the configurations are the same, it would be a diastereomer of the (2S,4S) or (2R,4R) isomers.
+   The key point is that the reduction of the symmetric ketone leads to a mixture of *endo* and *exo* products.
+Now, let's combine the products and analyze the HPLC results.
+**Combining the Products:**
+From Reaction I: (S)-5-methoxy-3-hydroxycaproic acid
+From Reaction II: A mixture of reduction products at C2 and C4.
+Let's focus on the symmetry of the molecules. The reduction of the symmetric pentane-2,4-dione can lead to enantiomers or diastereomers at the C2 and C4 centers after acidic workup.
+Consider the possible diastereomers of the reduction products of pentane-2,4-dione:
+- **Both *endo*:** (2S,4S)-1-hydroxy-2,4-dihydroxypentanoic acid
+- **Both *exo*:** (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid
+- **One *endo*, one *exo*:**
+   - If the configurations are opposite, e.g., (2S,4R)- or (2R,4S), the compounds are enantiomers of each other.
+   - If the configurations are the same, e.g., (2S,4S) or (2R,4R), they are diastereomers.
+The important aspect is that the reduction of the symmetric dione leads to a pair of enantiomers or a pair of diastereomers at the reduced positions.
+**Analyzing the Chromatograms:**
+- **Normal-phase HPLC:** This separates molecules based on their size and polarity. The two reduction products from pentane-2,4-dione will elute as a pair due to their similar size and polarity. The (S)-product from reaction I will also elute separately. So, in addition to the pair from the dione reduction, we have the individual peak for the (S)-product. This gives us 2 peaks from the dione reduction (the pair) and 1 peak for the (S)-product, totaling 3 peaks.
+- **Chiral HPLC:** This separates enantiomers. If the reduction products of pentane-2,4-dione are enantiomers ((2S,4S) and (2R,4R)), they will be resolved into two peaks. The (S)-product from reaction I is not an enantiomer of the dione reduction products. Therefore, the chiral HPLC will show 2 peaks from the dione reduction (the enantiomers) and 1 peak for the (S)-product, totaling 3 peaks.
+However, let's reconsider the outcome of reaction II. The reduction of a symmetric ketone with excess NaBH4 typically leads to a pair of enantiomers at the reduced center.
+So, the products from reaction II, after acidic workup, will be a pair of enantiomers, e.g., (2S,4S)- and (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid.
+**Combining the sets of products:**
+- From Reaction I: (S)-5-methoxy-3-hydroxycaproic acid
+- From Reaction II: (2S,4S)- and (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid
+Now let's consider the chiral HPLC. The chiral stationary phase will separate enantiomers.
+- The (S)-product from reaction I is not enantiometrically pure; it's a single enantiomer.
+- The products from reaction II are a pair of enantiomers.
+When you mix these products and run them on chiral HPLC:
+- The (S)-product from reaction I will form a peak.
+- The pair of enantiomers from reaction II will be separated into two peaks.
+So, on chiral HPLC, we expect 1 peak for the (S)-product and 2 peaks for the enantiomers of the dione reduction product, totaling 3 peaks.
+Let's verify the logic. The core question is about the number of peaks observed.
+**Normal-phase HPLC:**
+- Peak 1: (S)-5-methoxy-3-hydroxycaproic acid
+- Peak 2-3: The pair of reduction products from pentane-2,4-dione (whatever the exact stereochemistry, they will elute together due to similar properties).
+Total peaks = 3.
+**Chiral HPLC:**
+- Peak 1: (S)-5-methoxy-3-hydroxycaproic acid
+- Peak 2: (2S,4S)-1-hydroxy-2,4-dihydroxypentanoic acid
+- Peak 3: (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid
+Total peaks = 3.
+Let's think about the possibilities for the reduction of pentane-2,4-dione with excess NaBH4. The *endo* rule often applies in reductions like this, leading to a pair of enantiomers.
+Consider the structure of pentane-2,4-dione: CH3-C(=O)-CH(CH3)2-C(=O)-CH3
+Reduction at C2: The hydrogen will add to the same face as the larger group (CH3), leading to a *endo* product with the hydroxyl group on the same face as one CH3. The other face will have the other CH3 group.
+Reduction at C4: Similarly, the hydrogen will add to the same face as the larger group (CH3), leading to a *endo* product with the hydroxyl group on the same face as one CH3. The other face will have the other CH3 group.
+The two reductions are independent. The overall product will be a pair of enantiomers, (2S,4S) and (2R,4R), with various substituents.
+The key is that the reduction of the symmetric dione leads to a pair of enantiomers at the reduced centers.
+**Final thought process:**
+- Reaction I produces a single enantiomer ((S)-configuration preserved through reduction and workup).
+- Reaction II, involving the reduction of a symmetric ketone with excess NaBH4, will produce a pair of enantiomers at the reduced centers (C2 and C4).
+- The acidic workup will solidify the stereochemistry of these reduction products.
+- When the products are combined, we have one enantiomer from reaction I and a pair of enantiomers from reaction II.
+- On normal-phase HPLC, the three products will elute as three distinct peaks.
+- On chiral HPLC, the (S)-product from reaction I will form one peak, and the pair of enantiomers from reaction II will form two additional peaks.
+Therefore, the total number of peaks observed on normal-phase HPLC is 3. The total number of peaks observed on chiral HPLC is also 3.
+Let's confirm the expected products and their stereochemistry.
+**Expected products:**
+- **Reaction I:** (S)-5-methoxy-3-hydroxycaproic acid
+- **Reaction II:** A mixture of reduction products. The key is the *endo* reduction, leading to (2S,4S) and (2R,4R) isomers after acidic workup.
+**Chiral HPLC analysis of the mixture:**
+- The (S)-product from reaction I is not enantiometrically pure regarding the new centers formed in reaction II.
+- The products from reaction II are a pair of enantiomers at the reduced centers.
+When these are mixed and analyzed on chiral HPLC:
+- The (S)-product from reaction I will likely form a single peak, as the chiral HPLC is designed to separate enantiomers, and this product is not one of them.
+- The pair of enantiomers from reaction II will be separated into two peaks.
+This seems inconsistent with the initial thought. Let's backtrack.
+The reduction of pentane-2,4-dione with excess NaBH4 will lead to a pair of enantiomers at the reduced centers. The acidic workup will confirm this. The products from reaction II will therefore be (2S,4S)- and (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid.
+**Combining the products:**
+- (S)-5-methoxy-3-hydroxycaproic acid
+- (2S,4S)-1-hydroxy-2,4-dihydroxypentanoic acid
+- (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid
+**Normal-phase HPLC:**  Three distinct products, eluting as three peaks.
+**Chiral HPLC:**
+- The (S)-product from reaction I.
+- The (2S,4S) enantiomer from reaction II.
+- The (2R,4R) enantiomer from reaction II.
+The chiral HPLC will separate the enantiomers of the dione reduction product. The (S)-product from reaction I is not an enantiomer of the dione reduction products. Therefore, we expect 1 peak for the (S)-product, 1 peak for the (2S,4S) enantiomer, and 1 peak for the (2R,4R) enantiomer.
+**Re-evaluation:**
+The question asks for the number of peaks observed in the chromatograms.
+**Normal-phase HPLC:**  The three products will elute as three distinct peaks. So, 3 peaks.
+**Chiral HPLC:** The (S)-product is a single enantiomer. The products from reaction II are a pair of enantiomers. When these are analyzed on chiral HPLC, the (S)-product will form one peak, and the pair of enantiomers from reaction II will be separated into two peaks. So, 3 peaks in total.
+Let's consider the possibility of meso forms or other complications. The reduction of symmetric ketones with excess NaBH4 typically leads to enantiomers.
+If the product of reaction II was a meso compound, it would be optically inactive. However, the reduction step introduces chirality.
+The progress of the reactions is monitored using TLC, and they are 100% complete. This implies clean products.
+**Final reasoning:**
+- **Reaction I:** Reduces the ketone to an alcohol, maintaining the (S) configuration. Acidic workup gives the carboxylic acid.
+- **Reaction II:** Excess NaBH4 reduces both ketones to alcohols. The *endo* reduction is likely, leading to a pair of enantiomers at the reduced centers.
+- **Combined Products:**  We have one enantiomer from reaction I and a pair of enantiomers from reaction II.
+- **Normal-phase HPLC:**  Three distinct peaks (the three products).
+- **Chiral HPLC:**  The (S)-product forms one peak. The pair of enantiomers from reaction II are separated into two peaks. Total peaks = 3.
+The key insight is that the reduction of the symmetric pentane-2,4-dione leads to a pair of enantiomers, even with excess NaBH4. The *endo* rule still applies in this case.
+Consider the structure of the dione reduction products:  The hydroxyl groups can rotate. The *endo* product has the hydroxyl group on the same face as one methyl group. The *exo* product has it on the opposite face. For a symmetric ketone, these are enantiomers upon reduction.
+The (S)-product from reaction I is not enantiometrically pure regarding the new stereochemistry introduced by the reduction and workup of the dione.
+When the products are combined and run on chiral HPLC:
+- The (S)-product will form one peak.
+- The pair of enantiomers from reaction II will be separated into two peaks.
+This leads to a total of 3 peaks on chiral HPLC. The question asks for the number of peaks observed in *both* chromatograms.
+On normal-phase HPLC, the three distinct products will elute as three peaks.
+Therefore, the number of peaks observed in the normal-phase HPLC chromatogram is 3, and the number of peaks observed in the chiral HPLC chromatogram is 3.
+&lt;|im_start|&gt;answer
+Solution:
+Reaction I involves the reduction of (S)-5-methoxyhexan-3-one with LAH followed by an acidic workup. LAH reduces the ketone group to a primary alcohol. The resulting (S)-3-hydroxyhexan-5-ol, upon acidic workup, forms a carbocation at the C3 position. This carbocation is planar due to the conjugated system and retains the (S) configuration.
+Reaction II involves the treatment of pentane-2,4-dione with excess NaBH4 followed by an acidic workup. NaBH4 reduces the carbonyl groups to primary alcohols. The reduction of the symmetric ketone leads to a pair of enantiomers at the reduced centers (C2 and C4) due to the *endo* rule. The acidic workup confirms this, yielding a mixture of (2S,4S)- and (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid.
+When the products from both reactions are combined, we have:
+- From Reaction I: (S)-5-methoxy-3-hydroxycaproic acid
+- From Reaction II: (2S,4S)- and (2R,4R)-1-hydroxy-2,4-dihydroxypentanoic acid
+**Normal-phase HPLC:**
+The normal-phase HPLC separates the products based on their size and polarity. The two reduction products from pentane-2,4-dione are structurally similar and will elute as a pair. The (S)-product from reaction I is distinct. Therefore, the chromatogram will show 3 peaks: one for the (S)-product and two for the pair of reduction products.
+**Chiral HPLC:**
+The chiral stationary phase separates enantiomers. The (S)-5-methoxy-3-hydroxycaproic acid is a single enantiomer. The reduction products of pentane-2,4-dione are a pair of enantiomers. Thus, the chiral HPLC chromatogram will show 1 peak for the (S)-product and 2 peaks for the enantiomers of the dione reduction product.
+The question asks for the number of peaks observed in the chromatograms. For each chromatography type, we need to count the number of distinct peaks.
+**Normal-phase HPLC:**  The three products lead to 3 peaks.
+**Chiral HPLC:** The (S)-product and the pair of enantiomers lead to 3 peaks (1 + 2).
+Final Answer: The final answer is $\boxed{6}$</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">

</xml_diff>